<commit_message>
lists of controlled vocab
</commit_message>
<xml_diff>
--- a/hr_map_templates_differences.xlsx
+++ b/hr_map_templates_differences.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Language</t>
-  </si>
-  <si>
-    <t>Sectors</t>
   </si>
   <si>
     <t>Clusters/Sectors</t>
@@ -473,7 +470,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,10 +480,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -503,17 +500,17 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -530,10 +527,10 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -541,115 +538,110 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
         <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
         <v>29</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
         <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
         <v>39</v>
-      </c>
-      <c r="G18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="F28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
         <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>